<commit_message>
Problem 4(a) by hand
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 01/HW 1 Scratch Work.xlsx
+++ b/03 - Homework/HW 01/HW 1 Scratch Work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="11_F25DC773A252ABDACC1048C6B19D63485ADE58F3" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B4976DAA-9D70-4112-A1D6-7F2D83B502BC}"/>
+  <xr:revisionPtr revIDLastSave="356" documentId="11_F25DC773A252ABDACC1048C6B19D63485ADE58F3" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5691F1A5-EF74-4C64-B1A2-F3687D7258CE}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="-120" windowWidth="15075" windowHeight="14805" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Gregor</t>
   </si>
@@ -155,7 +155,16 @@
     </r>
   </si>
   <si>
-    <t>?????</t>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>At least one is a truth teller</t>
+  </si>
+  <si>
+    <t>No one is a truth teller</t>
+  </si>
+  <si>
+    <t>Or</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -307,6 +316,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K18"/>
+  <dimension ref="B2:O18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +621,7 @@
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>8</v>
       </c>
@@ -619,7 +629,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -627,7 +637,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -635,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,8 +670,17 @@
       <c r="K5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="b">
         <v>1</v>
       </c>
@@ -691,8 +710,20 @@
         <f>AND(I6:J6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M6" t="b">
+        <f>COUNTIFS($B6:$D6, TRUE) &gt;= 1</f>
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <f>COUNTIFS($B6:$D6, TRUE) = 0</f>
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <f>OR(M6:N6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="b">
         <v>1</v>
       </c>
@@ -723,8 +754,20 @@
         <f t="shared" ref="K7:K13" si="4">AND(I7:J7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M7" t="b">
+        <f t="shared" ref="M7:M13" si="5">COUNTIFS($B7:$D7, TRUE) &gt;= 1</f>
+        <v>1</v>
+      </c>
+      <c r="N7" t="b">
+        <f t="shared" ref="N7:N13" si="6">COUNTIFS($B7:$D7, TRUE) = 0</f>
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" ref="O7:O13" si="7">OR(M7:N7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="b">
         <v>1</v>
       </c>
@@ -732,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="3" t="b">
-        <f t="shared" ref="D8:D13" si="5">NOT(D7)</f>
+        <f t="shared" ref="D8:D13" si="8">NOT(D7)</f>
         <v>1</v>
       </c>
       <c r="F8" s="3" t="b">
@@ -755,8 +798,20 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M8" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="b">
         <v>1</v>
       </c>
@@ -764,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F9" t="b">
@@ -787,8 +842,20 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N9" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" t="b">
         <f>NOT(B6)</f>
         <v>0</v>
@@ -797,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F10" t="b">
@@ -820,17 +887,29 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N10" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="b">
-        <f t="shared" ref="B11:B13" si="6">NOT(B7)</f>
+        <f t="shared" ref="B11:B13" si="9">NOT(B7)</f>
         <v>0</v>
       </c>
       <c r="C11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E11" s="8"/>
@@ -855,17 +934,29 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M11" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N11" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F12" t="b">
@@ -888,17 +979,29 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M12" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N12" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="b">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F13" t="b">
@@ -921,8 +1024,25 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M13" t="b">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -949,11 +1069,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D40DE64-D92C-4150-AE99-995FF1CD1D4E}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1029,11 +1147,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>